<commit_message>
fixed names of parent/child classes
working on making it output to a file and will prob have it done tomorrow
</commit_message>
<xml_diff>
--- a/CMPS 340 project/Doc/TaskProgresReport.xlsx
+++ b/CMPS 340 project/Doc/TaskProgresReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drewh\Desktop\CMPS 340 project\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAAE9CC-BEAB-403A-9612-CA2D555544EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082B9BBC-773F-4464-8FDA-612A726D9D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Task Name</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Rex Liner</t>
+  </si>
+  <si>
+    <t>PA2</t>
   </si>
 </sst>
 </file>
@@ -381,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,6 +454,20 @@
         <v>10</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>45616</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>